<commit_message>
reduce tasks and metrics
</commit_message>
<xml_diff>
--- a/doc/test/Metrics.xlsx
+++ b/doc/test/Metrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GoogleDriveMirror\UNI\Thesis\Files\doc\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32545070-E306-46E8-B805-3618E7E2FF1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3540D747-AF6E-4DD1-8D50-73DC243667DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{54B71262-651B-4420-9EBC-D966CD7E177D}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{54B71262-651B-4420-9EBC-D966CD7E177D}"/>
   </bookViews>
   <sheets>
     <sheet name="LLM_Edge_Metrics_Combined" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="81">
   <si>
     <t>Category</t>
   </si>
@@ -196,24 +196,6 @@
     <t>Text overlap with references</t>
   </si>
   <si>
-    <t>Human Evaluation</t>
-  </si>
-  <si>
-    <t>Likert scale (fluency, coherence, etc.)</t>
-  </si>
-  <si>
-    <t>Zero-Shot Accuracy</t>
-  </si>
-  <si>
-    <t>Accuracy with no task-specific training</t>
-  </si>
-  <si>
-    <t>Cosine Similarity</t>
-  </si>
-  <si>
-    <t>Vector space comparison</t>
-  </si>
-  <si>
     <t>Privacy</t>
   </si>
   <si>
@@ -272,6 +254,15 @@
   </si>
   <si>
     <t>Transferability across devices</t>
+  </si>
+  <si>
+    <t>Simple generic metric</t>
+  </si>
+  <si>
+    <t>Need for root</t>
+  </si>
+  <si>
+    <t>Quality</t>
   </si>
 </sst>
 </file>
@@ -1236,10 +1227,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C87073B9-E32D-41DE-973D-04F880442274}">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1247,9 +1238,10 @@
     <col min="1" max="1" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1259,8 +1251,11 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
@@ -1270,8 +1265,9 @@
       <c r="C2" s="8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="8"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -1281,8 +1277,9 @@
       <c r="C3" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
@@ -1292,8 +1289,9 @@
       <c r="C4" s="8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
@@ -1303,8 +1301,9 @@
       <c r="C5" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="8"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
@@ -1314,8 +1313,9 @@
       <c r="C6" s="8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="8"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>3</v>
       </c>
@@ -1325,8 +1325,9 @@
       <c r="C7" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>3</v>
       </c>
@@ -1336,8 +1337,9 @@
       <c r="C8" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>3</v>
       </c>
@@ -1347,8 +1349,9 @@
       <c r="C9" s="8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>3</v>
       </c>
@@ -1358,8 +1361,9 @@
       <c r="C10" s="8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>22</v>
       </c>
@@ -1369,8 +1373,9 @@
       <c r="C11" s="10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="10"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>22</v>
       </c>
@@ -1380,8 +1385,9 @@
       <c r="C12" s="10" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="10"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>27</v>
       </c>
@@ -1391,8 +1397,9 @@
       <c r="C13" s="12" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="12"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>27</v>
       </c>
@@ -1402,8 +1409,9 @@
       <c r="C14" s="12" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="12"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>27</v>
       </c>
@@ -1413,8 +1421,9 @@
       <c r="C15" s="12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="12"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>27</v>
       </c>
@@ -1424,8 +1433,9 @@
       <c r="C16" s="12" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="12"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>27</v>
       </c>
@@ -1435,8 +1445,9 @@
       <c r="C17" s="12" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="12"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>27</v>
       </c>
@@ -1446,8 +1457,9 @@
       <c r="C18" s="12" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="12"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>27</v>
       </c>
@@ -1457,8 +1469,9 @@
       <c r="C19" s="12" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="12"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>42</v>
       </c>
@@ -1468,8 +1481,9 @@
       <c r="C20" s="5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>42</v>
       </c>
@@ -1479,8 +1493,9 @@
       <c r="C21" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="5"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>42</v>
       </c>
@@ -1490,10 +1505,11 @@
       <c r="C22" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="5"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="B23" s="13" t="s">
         <v>50</v>
@@ -1501,10 +1517,11 @@
       <c r="C23" s="14" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="14"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="B24" s="13" t="s">
         <v>52</v>
@@ -1512,10 +1529,11 @@
       <c r="C24" s="14" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="14"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="B25" s="13" t="s">
         <v>54</v>
@@ -1523,10 +1541,11 @@
       <c r="C25" s="14" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" s="14"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="B26" s="13" t="s">
         <v>56</v>
@@ -1534,138 +1553,127 @@
       <c r="C26" s="14" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" s="14"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="C27" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" s="14"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="B28" s="15" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="13" t="s">
+      <c r="C28" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="D28" s="16"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="15" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" s="13" t="s">
+      <c r="C29" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="D29" s="16"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="15" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
+      <c r="C30" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="D30" s="16"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C30" s="16" t="s">
+      <c r="C31" s="16" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="B31" s="15" t="s">
+      <c r="D31" s="16"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="16" t="s">
+      <c r="B32" s="17" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="B32" s="15" t="s">
+      <c r="C32" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="D32" s="18"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" s="17" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="B33" s="15" t="s">
+      <c r="C33" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="C33" s="16" t="s">
+      <c r="D33" s="18"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="17" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="17" t="s">
+      <c r="C34" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="D34" s="18"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C35" s="18" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="B35" s="17" t="s">
+      <c r="D35" s="18"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="C35" s="18" t="s">
+      <c r="C36" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="B36" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="C36" s="18" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="B37" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="C37" s="18" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="B38" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="C38" s="18" t="s">
-        <v>83</v>
-      </c>
+      <c r="D36" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>